<commit_message>
update: språkvask QField app
</commit_message>
<xml_diff>
--- a/docs/source/app_instructions/tbl/QField_treregisterinsapp_attribute_design.xlsx
+++ b/docs/source/app_instructions/tbl/QField_treregisterinsapp_attribute_design.xlsx
@@ -367,7 +367,7 @@
     <t xml:space="preserve">Default: 15-20%</t>
   </si>
   <si>
-    <t xml:space="preserve">VAT19 variabler</t>
+    <t xml:space="preserve">VAT variabler</t>
   </si>
   <si>
     <t xml:space="preserve">Alder</t>
@@ -594,8 +594,8 @@
   </sheetPr>
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="F:H"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1399,7 +1399,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
         <v>44</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
         <v>45</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
         <v>46</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <v>47</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <v>48</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <v>49</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
         <v>50</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
         <v>51</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
         <v>52</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
         <v>53</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
         <v>54</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
         <v>55</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
         <v>56</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
         <v>57</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
         <v>58</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
         <v>59</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
         <v>60</v>
       </c>

</xml_diff>